<commit_message>
Adiciona modelagem e scripts spmedgroup
</commit_message>
<xml_diff>
--- a/Project_spmedgruop/Modelo_Descritivos.xlsx
+++ b/Project_spmedgruop/Modelo_Descritivos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\47651807863\Desktop\MyRepository\Project_spmedgruop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFDA10A-3109-497D-AEA8-44E98D13C50E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1124E6-27A6-4B7D-BCA7-EF21F56C2715}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{6B3045F8-3B33-4B2D-B04E-E2BDBC4F2986}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="38">
   <si>
     <t>TipoUsuario</t>
   </si>
@@ -121,6 +121,24 @@
   </si>
   <si>
     <t>Descrição</t>
+  </si>
+  <si>
+    <t>Situacao</t>
+  </si>
+  <si>
+    <t>IDSituacao</t>
+  </si>
+  <si>
+    <t>TituloSituacao</t>
+  </si>
+  <si>
+    <t>Cancelada</t>
+  </si>
+  <si>
+    <t>Realizada</t>
+  </si>
+  <si>
+    <t>Agendada</t>
   </si>
 </sst>
 </file>
@@ -136,7 +154,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,6 +185,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -180,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -192,16 +228,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -218,6 +245,27 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,14 +582,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD38FB72-E1D2-4744-82CD-D190ADB36146}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
@@ -549,217 +598,216 @@
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4"/>
+      <c r="D1" s="13"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="5"/>
+      <c r="G1" s="4"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="L1" s="4" t="s">
+      <c r="J1" s="12"/>
+      <c r="L1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="4"/>
+      <c r="M1" s="13"/>
       <c r="N1" s="1"/>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="4"/>
+      <c r="P1" s="13"/>
       <c r="Q1" s="1"/>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="7"/>
+      <c r="S1" s="14"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="8"/>
+      <c r="D2" s="5"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="L2" s="8" t="s">
+      <c r="J2" s="6"/>
+      <c r="L2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="8"/>
+      <c r="M2" s="5"/>
       <c r="N2" s="2"/>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="8"/>
+      <c r="P2" s="5"/>
       <c r="Q2" s="2"/>
-      <c r="R2" s="8" t="s">
+      <c r="R2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="8"/>
+      <c r="S2" s="5"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="D3" s="7"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="13"/>
+      <c r="G3" s="10"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="14"/>
-      <c r="L3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="13"/>
+      <c r="J3" s="11"/>
+      <c r="L3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="10"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="P3" s="10"/>
+      <c r="P3" s="7"/>
       <c r="Q3" s="2"/>
-      <c r="R3" s="13" t="s">
+      <c r="R3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="13"/>
+      <c r="S3" s="10"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="2"/>
       <c r="F4" s="10" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="12"/>
-      <c r="L4" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="M4" s="13"/>
+      <c r="J4" s="9"/>
+      <c r="L4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="10"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="13" t="s">
+      <c r="R4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="S4" s="13"/>
+      <c r="S4" s="10"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="10"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="11"/>
+      <c r="F5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="7"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="12"/>
-      <c r="L5" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="13"/>
+      <c r="J5" s="9"/>
+      <c r="L5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="7"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
-      <c r="R5" s="10" t="s">
+      <c r="R5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="S5" s="10"/>
+      <c r="S5" s="7"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="10"/>
+      <c r="F6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="8"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="12"/>
-      <c r="L6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="M6" s="10"/>
+      <c r="J6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="7"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
-      <c r="R6" s="10" t="s">
+      <c r="R6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="S6" s="10"/>
+      <c r="S6" s="7"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="F7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="7"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="10"/>
+      <c r="J7" s="9"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
-      <c r="R7" s="10" t="s">
+      <c r="R7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="S7" s="10"/>
+      <c r="S7" s="7"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
@@ -780,8 +828,10 @@
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="C9" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="15"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -798,8 +848,12 @@
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="C10" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>34</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -816,8 +870,12 @@
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="C11" s="16">
+        <v>1</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>35</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="H11" s="2"/>
@@ -833,8 +891,12 @@
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="C12" s="16">
+        <v>2</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="H12" s="2"/>
@@ -850,8 +912,12 @@
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="C13" s="16">
+        <v>3</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>37</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="H13" s="2"/>
@@ -863,7 +929,8 @@
       <c r="P13" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="C9:D9"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="C1:D1"/>

</xml_diff>